<commit_message>
UI Updated with SP
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\BCC\NewWeb\MemberMIS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
@@ -17,9 +12,9 @@
     <sheet name="Member Import" sheetId="3" r:id="rId3"/>
     <sheet name="Data Export" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="180">
   <si>
     <t>SHG Monitoring System</t>
   </si>
@@ -550,12 +545,122 @@
   <si>
     <t>Required Sl No in First Column</t>
   </si>
+  <si>
+    <t>usp_GetGroup</t>
+  </si>
+  <si>
+    <t>usp_InsertVoucher</t>
+  </si>
+  <si>
+    <t>VouPurpId=1</t>
+  </si>
+  <si>
+    <t>VouPurpId=2</t>
+  </si>
+  <si>
+    <t>usp_GetPurpose</t>
+  </si>
+  <si>
+    <t>TypeCd=1/2</t>
+  </si>
+  <si>
+    <t>usp_UpdtGroupStaff</t>
+  </si>
+  <si>
+    <t>(For Admin User)</t>
+  </si>
+  <si>
+    <t>Staff Name</t>
+  </si>
+  <si>
+    <t>usp_GetStaffName</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Export </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Sl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Field from Query</t>
+    </r>
+  </si>
+  <si>
+    <t>VouPurpId=6</t>
+  </si>
+  <si>
+    <t>usp_GetCasBankFig</t>
+  </si>
+  <si>
+    <t>usp_ViewCashBook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receipt </t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Opening</t>
+  </si>
+  <si>
+    <t>Sub Total</t>
+  </si>
+  <si>
+    <t>Closing</t>
+  </si>
+  <si>
+    <t>Cash Book For The Period 01-03-2024 To 31-03-2024</t>
+  </si>
+  <si>
+    <t>Group Name: MATALA MAHILA BIKASH</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,8 +714,26 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -626,6 +749,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -666,7 +795,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -704,15 +833,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -729,6 +849,26 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,17 +888,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -792,7 +922,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -800,36 +929,12 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:depthPercent val="100"/>
       <c:rAngAx val="1"/>
     </c:view3D>
     <c:floor>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -840,7 +945,6 @@
       </c:spPr>
     </c:floor>
     <c:sideWall>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -851,7 +955,6 @@
       </c:spPr>
     </c:sideWall>
     <c:backWall>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -866,7 +969,6 @@
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -891,7 +993,6 @@
             <a:effectLst/>
             <a:sp3d/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -922,13 +1023,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
@@ -990,7 +1085,6 @@
             <a:effectLst/>
             <a:sp3d/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -1021,13 +1115,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
@@ -1066,28 +1154,20 @@
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="462258560"/>
-        <c:axId val="462264440"/>
+        <c:axId val="100225408"/>
+        <c:axId val="100226944"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="462258560"/>
+        <c:axId val="100225408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1116,19 +1196,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="462264440"/>
+        <c:crossAx val="100226944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="462264440"/>
+        <c:axId val="100226944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1146,7 +1224,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1175,7 +1252,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="462258560"/>
+        <c:crossAx val="100225408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1194,12 +1271,11 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.12536964129483816"/>
-          <c:y val="0.89409667541557303"/>
+          <c:y val="0.89409667541557314"/>
           <c:w val="0.77148293963254588"/>
           <c:h val="7.8125546806649168E-2"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1230,7 +1306,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1259,7 +1334,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1267,17 +1342,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1306,7 +1371,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1314,36 +1378,12 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:depthPercent val="100"/>
       <c:rAngAx val="1"/>
     </c:view3D>
     <c:floor>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1354,7 +1394,6 @@
       </c:spPr>
     </c:floor>
     <c:sideWall>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1365,7 +1404,6 @@
       </c:spPr>
     </c:sideWall>
     <c:backWall>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1380,7 +1418,6 @@
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1394,7 +1431,6 @@
             <a:effectLst/>
             <a:sp3d/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -1425,13 +1461,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
@@ -1482,7 +1512,6 @@
             <a:effectLst/>
             <a:sp3d/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -1513,13 +1542,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
@@ -1558,28 +1581,20 @@
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="216241256"/>
-        <c:axId val="216240472"/>
+        <c:axId val="100248960"/>
+        <c:axId val="101061760"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="216241256"/>
+        <c:axId val="100248960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1608,19 +1623,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216240472"/>
+        <c:crossAx val="101061760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216240472"/>
+        <c:axId val="101061760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1638,7 +1651,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1667,7 +1679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216241256"/>
+        <c:crossAx val="100248960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1682,7 +1694,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1713,7 +1724,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1742,7 +1752,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2924,7 +2934,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2959,7 +2969,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3136,22 +3146,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J119"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
@@ -3164,17 +3174,17 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3192,7 +3202,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -3203,7 +3213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -3211,7 +3221,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -3219,7 +3229,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -3236,7 +3246,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -3253,7 +3263,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -3261,8 +3271,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="9" spans="1:6">
+      <c r="A9" s="33">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -3275,51 +3285,51 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="17" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="17" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="17" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -3333,7 +3343,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -3344,7 +3354,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -3352,7 +3362,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="4">
         <v>1</v>
       </c>
@@ -3360,17 +3370,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="4">
         <v>2</v>
       </c>
@@ -3378,7 +3388,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="C24" s="15" t="s">
         <v>124</v>
       </c>
@@ -3393,7 +3403,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="C25" s="8" t="s">
         <v>127</v>
       </c>
@@ -3404,7 +3414,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="C26" s="8" t="s">
         <v>123</v>
       </c>
@@ -3415,7 +3425,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="C27" s="8" t="s">
         <v>128</v>
       </c>
@@ -3426,7 +3436,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="C28" s="8" t="s">
         <v>24</v>
       </c>
@@ -3435,25 +3445,25 @@
       <c r="F28" s="8"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="B31" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="23"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="20"/>
+    </row>
+    <row r="32" spans="1:7">
       <c r="B32" s="12"/>
       <c r="C32" s="15" t="s">
         <v>32</v>
@@ -3464,48 +3474,48 @@
       <c r="E32" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="F32" s="23"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F32" s="20"/>
+    </row>
+    <row r="33" spans="2:10">
       <c r="B33" s="12"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="14"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10">
       <c r="B34" s="12"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="14"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10">
       <c r="B35" s="12"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="14"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10">
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="14"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10">
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="14"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10">
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="14"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10">
       <c r="H41" s="1">
         <f>ROUND(I42/I41*100,2)</f>
         <v>86.36</v>
@@ -3517,7 +3527,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10">
       <c r="H42" s="1">
         <f>ROUND(J42/J41*100,2)</f>
         <v>95.45</v>
@@ -3529,7 +3539,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10">
       <c r="H45" s="1">
         <f>ROUND(I46/I45*100,2)</f>
         <v>90.91</v>
@@ -3541,7 +3551,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10">
       <c r="H46" s="1">
         <f>ROUND(J46/J45*100,2)</f>
         <v>86.36</v>
@@ -3553,11 +3563,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10">
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="4">
         <v>3</v>
       </c>
@@ -3565,7 +3575,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="4">
         <v>4</v>
       </c>
@@ -3573,7 +3583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="4">
         <v>5</v>
       </c>
@@ -3581,11 +3591,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="4"/>
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" s="4">
         <v>6</v>
       </c>
@@ -3593,7 +3603,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="4">
         <v>7</v>
       </c>
@@ -3601,12 +3611,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="C60" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="C61" s="1" t="s">
         <v>16</v>
       </c>
@@ -3614,24 +3624,28 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D62" s="27" t="s">
+    <row r="62" spans="1:5">
+      <c r="A62" s="34"/>
+      <c r="D62" s="24" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="B63" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="B64" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="25" t="s">
+    <row r="66" spans="1:6">
+      <c r="A66" s="22" t="s">
         <v>139</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -3648,8 +3662,8 @@
       </c>
       <c r="F66" s="13"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="24"/>
+    <row r="67" spans="1:6">
+      <c r="A67" s="21"/>
       <c r="B67" s="9"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7" t="s">
@@ -3658,8 +3672,8 @@
       <c r="E67" s="7"/>
       <c r="F67" s="14"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="24"/>
+    <row r="68" spans="1:6">
+      <c r="A68" s="21"/>
       <c r="B68" s="9"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7" t="s">
@@ -3668,8 +3682,8 @@
       <c r="E68" s="7"/>
       <c r="F68" s="14"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="24"/>
+    <row r="69" spans="1:6">
+      <c r="A69" s="21"/>
       <c r="B69" s="9"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7" t="s">
@@ -3678,8 +3692,8 @@
       <c r="E69" s="7"/>
       <c r="F69" s="14"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="24"/>
+    <row r="70" spans="1:6">
+      <c r="A70" s="21"/>
       <c r="B70" s="9"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7" t="s">
@@ -3688,8 +3702,8 @@
       <c r="E70" s="7"/>
       <c r="F70" s="14"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="24"/>
+    <row r="71" spans="1:6">
+      <c r="A71" s="21"/>
       <c r="B71" s="9"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7" t="s">
@@ -3698,8 +3712,8 @@
       <c r="E71" s="7"/>
       <c r="F71" s="14"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="24"/>
+    <row r="72" spans="1:6">
+      <c r="A72" s="21"/>
       <c r="B72" s="9"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7" t="s">
@@ -3708,8 +3722,8 @@
       <c r="E72" s="7"/>
       <c r="F72" s="14"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="24"/>
+    <row r="73" spans="1:6">
+      <c r="A73" s="21"/>
       <c r="B73" s="9"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7" t="s">
@@ -3718,8 +3732,8 @@
       <c r="E73" s="7"/>
       <c r="F73" s="14"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="24"/>
+    <row r="74" spans="1:6">
+      <c r="A74" s="21"/>
       <c r="B74" s="9"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7" t="s">
@@ -3728,8 +3742,8 @@
       <c r="E74" s="7"/>
       <c r="F74" s="14"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="24"/>
+    <row r="75" spans="1:6">
+      <c r="A75" s="21"/>
       <c r="B75" s="9"/>
       <c r="C75" s="7" t="s">
         <v>24</v>
@@ -3738,220 +3752,505 @@
       <c r="E75" s="7"/>
       <c r="F75" s="14"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="26">
+    <row r="77" spans="1:6">
+      <c r="D77" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="34"/>
+      <c r="E78" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="34"/>
+      <c r="E79" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="23">
         <v>8</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B80" s="17" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C78" s="1" t="s">
+    <row r="81" spans="1:14">
+      <c r="C81" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C79" s="1" t="s">
+    <row r="82" spans="1:14">
+      <c r="C82" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="D82" s="6" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C81" s="1" t="s">
+      <c r="E82" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14">
+      <c r="C84" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D82" s="6" t="s">
+    <row r="85" spans="1:14">
+      <c r="A85" s="34"/>
+      <c r="D85" s="6" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="26">
+      <c r="E85" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14">
+      <c r="A87" s="23">
         <v>9</v>
       </c>
-      <c r="B84" s="20" t="s">
+      <c r="B87" s="17" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C85" s="1" t="s">
+    <row r="88" spans="1:14">
+      <c r="A88" s="23"/>
+      <c r="B88" s="17"/>
+      <c r="C88" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C86" s="1" t="s">
+    <row r="89" spans="1:14">
+      <c r="A89" s="23"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14">
+      <c r="A90" s="23"/>
+      <c r="B90" s="17"/>
+      <c r="D90" s="6"/>
+    </row>
+    <row r="91" spans="1:14">
+      <c r="C91" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="D91" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="E91" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C87" s="1" t="s">
+    <row r="92" spans="1:14">
+      <c r="C92" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C88" s="1" t="s">
+      <c r="E92" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14">
+      <c r="C93" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D89" s="6" t="s">
+    <row r="94" spans="1:14">
+      <c r="D94" s="6" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="26">
+      <c r="E94" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14">
+      <c r="A96" s="23">
         <v>10</v>
       </c>
-      <c r="B91" s="20" t="s">
+      <c r="B96" s="17" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C92" s="1" t="s">
+      <c r="G96" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="H96" s="29"/>
+      <c r="I96" s="29"/>
+      <c r="J96" s="29"/>
+      <c r="K96" s="29"/>
+      <c r="L96" s="29"/>
+      <c r="M96" s="29"/>
+      <c r="N96" s="29"/>
+    </row>
+    <row r="97" spans="1:14">
+      <c r="C97" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C93" s="1" t="s">
+      <c r="G97" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="H97" s="29"/>
+      <c r="I97" s="29"/>
+      <c r="J97" s="29"/>
+      <c r="K97" s="29"/>
+      <c r="L97" s="29"/>
+      <c r="M97" s="29"/>
+      <c r="N97" s="29"/>
+    </row>
+    <row r="98" spans="1:14">
+      <c r="C98" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C94" s="1" t="s">
+      <c r="G98" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="K98" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14">
+      <c r="C99" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D94" s="6" t="s">
+      <c r="D99" s="6" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D96" s="6" t="s">
+      <c r="E99" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H99" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I99" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="J99" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="K99" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="L99" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M99" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="N99" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14">
+      <c r="G100" s="28"/>
+      <c r="H100" s="28"/>
+      <c r="I100" s="28">
+        <v>10</v>
+      </c>
+      <c r="J100" s="28">
+        <v>50</v>
+      </c>
+      <c r="K100" s="28"/>
+      <c r="L100" s="28"/>
+      <c r="M100" s="28">
+        <v>10</v>
+      </c>
+      <c r="N100" s="28"/>
+    </row>
+    <row r="101" spans="1:14">
+      <c r="D101" s="6" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="26">
+      <c r="E101" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="G101" s="28"/>
+      <c r="H101" s="28"/>
+      <c r="I101" s="28">
+        <v>20</v>
+      </c>
+      <c r="J101" s="28">
+        <v>60</v>
+      </c>
+      <c r="K101" s="28"/>
+      <c r="L101" s="28"/>
+      <c r="M101" s="28">
+        <v>20</v>
+      </c>
+      <c r="N101" s="28"/>
+    </row>
+    <row r="102" spans="1:14">
+      <c r="D102" s="6"/>
+      <c r="E102" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="G102" s="28"/>
+      <c r="H102" s="28"/>
+      <c r="I102" s="28">
+        <v>30</v>
+      </c>
+      <c r="J102" s="28">
+        <v>70</v>
+      </c>
+      <c r="K102" s="28"/>
+      <c r="L102" s="28"/>
+      <c r="M102" s="28"/>
+      <c r="N102" s="28">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14">
+      <c r="A103" s="23">
         <v>11</v>
       </c>
-      <c r="B97" s="20" t="s">
+      <c r="B103" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="D97" s="6"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C98" s="1" t="s">
+      <c r="D103" s="6"/>
+      <c r="G103" s="28"/>
+      <c r="H103" s="28"/>
+      <c r="I103" s="28">
+        <v>40</v>
+      </c>
+      <c r="J103" s="28">
+        <v>80</v>
+      </c>
+      <c r="K103" s="28"/>
+      <c r="L103" s="28"/>
+      <c r="M103" s="28"/>
+      <c r="N103" s="28">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14">
+      <c r="C104" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D98" s="6" t="s">
+      <c r="D104" s="6" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="6"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D100" s="6" t="s">
+      <c r="E104" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G104" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="H104" s="7"/>
+      <c r="I104" s="7">
+        <f>SUM(I100:I103)</f>
+        <v>100</v>
+      </c>
+      <c r="J104" s="7">
+        <f>SUM(J100:J103)</f>
+        <v>260</v>
+      </c>
+      <c r="K104" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="L104" s="7"/>
+      <c r="M104" s="7">
+        <f>SUM(M100:M103)</f>
+        <v>30</v>
+      </c>
+      <c r="N104" s="7">
+        <f>SUM(N100:N103)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14">
+      <c r="D105" s="6"/>
+      <c r="G105" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="H105" s="27"/>
+      <c r="I105" s="27">
+        <v>300</v>
+      </c>
+      <c r="J105" s="27">
+        <v>500</v>
+      </c>
+      <c r="K105" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="L105" s="27"/>
+      <c r="M105" s="27">
+        <f>I106-M104</f>
+        <v>370</v>
+      </c>
+      <c r="N105" s="27">
+        <f>J106-N104</f>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14">
+      <c r="D106" s="6" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="4">
+      <c r="E106" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G106" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H106" s="7"/>
+      <c r="I106" s="7">
+        <f>I105+I104</f>
+        <v>400</v>
+      </c>
+      <c r="J106" s="7">
+        <f>J105+J104</f>
+        <v>760</v>
+      </c>
+      <c r="K106" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L106" s="7"/>
+      <c r="M106" s="7">
+        <f>M105+M104</f>
+        <v>400</v>
+      </c>
+      <c r="N106" s="7">
+        <f>N105+N104</f>
+        <v>760</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14">
+      <c r="A108" s="4">
         <v>12</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C103" s="1" t="s">
+    <row r="109" spans="1:14">
+      <c r="C109" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D103" s="6" t="s">
+      <c r="D109" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C104" s="1" t="s">
+    <row r="110" spans="1:14">
+      <c r="C110" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D104" s="6"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D105" s="27" t="s">
+      <c r="D110" s="6"/>
+    </row>
+    <row r="111" spans="1:14">
+      <c r="D111" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="1" t="s">
+    <row r="112" spans="1:14">
+      <c r="B112" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="1" t="s">
+    <row r="113" spans="1:5">
+      <c r="B113" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="1" t="s">
+    <row r="114" spans="1:5">
+      <c r="B114" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="1" t="s">
+    <row r="115" spans="1:5">
+      <c r="B115" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="4">
+    <row r="118" spans="1:5">
+      <c r="A118" s="4">
         <v>13</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C113" s="1" t="s">
+      <c r="C118" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="C119" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="4">
+    <row r="120" spans="1:5">
+      <c r="C120" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="D122" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="4">
         <v>14</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B123" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C117" s="1" t="s">
+    <row r="124" spans="1:5">
+      <c r="C124" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="4">
+    <row r="126" spans="1:5">
+      <c r="A126" s="4">
         <v>15</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B126" s="2" t="s">
         <v>154</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
+    <mergeCell ref="G97:N97"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="C31:E31"/>
+    <mergeCell ref="G96:N96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3960,7 +4259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3968,7 +4267,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" style="1" customWidth="1"/>
@@ -3978,7 +4277,7 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>31</v>
       </c>
@@ -3995,7 +4294,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4012,7 +4311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4029,7 +4328,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4046,7 +4345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4063,7 +4362,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4080,7 +4379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4097,7 +4396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4114,7 +4413,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4131,7 +4430,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4148,7 +4447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4172,7 +4471,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4180,7 +4479,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -4191,7 +4490,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
@@ -4214,7 +4513,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4231,7 +4530,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4248,7 +4547,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4268,7 +4567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4285,7 +4584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4305,7 +4604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4325,7 +4624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4345,7 +4644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4362,7 +4661,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4376,7 +4675,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4396,7 +4695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4416,7 +4715,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4433,7 +4732,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4450,7 +4749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4467,7 +4766,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4487,7 +4786,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4507,7 +4806,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4521,7 +4820,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4541,7 +4840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4555,7 +4854,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4572,7 +4871,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4592,7 +4891,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4612,7 +4911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -4632,7 +4931,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -4652,7 +4951,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -4675,7 +4974,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4683,7 +4982,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -4694,7 +4993,7 @@
     <col min="7" max="7" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>

</xml_diff>